<commit_message>
Updating database fields list
</commit_message>
<xml_diff>
--- a/TelscaleSMSCDBAnalysis.xlsx
+++ b/TelscaleSMSCDBAnalysis.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="298"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="741"/>
   </bookViews>
   <sheets>
-    <sheet name="LIVE" sheetId="1" r:id="rId1"/>
-    <sheet name="LIVE_SMS" sheetId="2" r:id="rId2"/>
-    <sheet name="ARCHIVE" sheetId="3" r:id="rId3"/>
-    <sheet name="SMS_ROUTING_RULE" sheetId="4" r:id="rId4"/>
+    <sheet name="CURRENT_SLOT_TABLE" sheetId="5" r:id="rId1"/>
+    <sheet name="DST_SLOT_TABLE_YYYY_MM_DD" sheetId="6" r:id="rId2"/>
+    <sheet name="SLOT_MESSAGES_TABLE_YYYY_MM_DD" sheetId="2" r:id="rId3"/>
+    <sheet name="MESSAGES_YYYY_MM_DD" sheetId="3" r:id="rId4"/>
+    <sheet name="SMS_ROUTING_RULE" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="119">
   <si>
     <t>Column Name</t>
   </si>
@@ -40,45 +41,21 @@
     <t>ADDR_DST_DIGITS</t>
   </si>
   <si>
-    <t>destination address digits</t>
-  </si>
-  <si>
     <t>ADDR_DST_TON</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
-    <t>destination smpp style type of number</t>
-  </si>
-  <si>
     <t>ADDR_DST_NPI</t>
   </si>
   <si>
-    <t>destination smpp style type of numbering plan indicator</t>
-  </si>
-  <si>
     <t>IN_SYSTEM</t>
   </si>
   <si>
-    <t>0-idle state, 1-waiting for delivering, 2-delivering in progress</t>
-  </si>
-  <si>
-    <t>IN_SYSTEM_DATE</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>date when smsSet becomes under “IN_SYSTEM” state (delivery start)</t>
-  </si>
-  <si>
-    <t>DUE_DATE</t>
-  </si>
-  <si>
-    <t>time when next delivery attempts must be done</t>
-  </si>
-  <si>
     <t>DUE_DELAY</t>
   </si>
   <si>
@@ -100,18 +77,6 @@
     <t>true if after SMSC was successfully registered at HLR after delivery failure</t>
   </si>
   <si>
-    <t xml:space="preserve">PRIMARY KEY (TARGET_ID) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE INDEX ON LIVE (IN_SYSTEM); </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE INDEX ON LIVE (DUE_DATE); </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE INDEX ON LIVE (IN_SYSTEM_DATE); </t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -133,9 +98,6 @@
     <t>bigint</t>
   </si>
   <si>
-    <t>unique message ID assigned by SMSC (since SMSC started)</t>
-  </si>
-  <si>
     <t>MO_MESSAGE_REF</t>
   </si>
   <si>
@@ -241,9 +203,6 @@
     <t>OPTIONAL_PARAMETERS</t>
   </si>
   <si>
-    <t>MAP&lt;int, blob&gt;</t>
-  </si>
-  <si>
     <t>TLVs</t>
   </si>
   <si>
@@ -259,27 +218,9 @@
     <t>The validity period of this message (if ESME have not defined or for MO messages this field is filled bu default SMSC settings)</t>
   </si>
   <si>
-    <t>LAST_DELIVERY</t>
-  </si>
-  <si>
-    <t>time of last delivery attempt (null if it were not attempts)</t>
-  </si>
-  <si>
     <t>DELIVERY_COUNT</t>
   </si>
   <si>
-    <t>delivery tries count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY KEY (ID) </t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (TARGET_ID);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (MESSAGE_ID);</t>
-  </si>
-  <si>
     <t>DEST_CLUSTER_NAME</t>
   </si>
   <si>
@@ -334,9 +275,6 @@
     <t>NNN_NP</t>
   </si>
   <si>
-    <t>ErrorCode value will be put here (0==success)</t>
-  </si>
-  <si>
     <t>SM_TYPE</t>
   </si>
   <si>
@@ -346,24 +284,6 @@
     <t>delivery tries count (this will be==1 if a message was delivered from a first step)</t>
   </si>
   <si>
-    <t>CREATE INDEX ON LIVE (ADDR_DST_DIGITS);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (ADDR_SRC_DIGITS);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (SM_TYPE);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (SM_STATUS);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (IN_SYSTEM);</t>
-  </si>
-  <si>
-    <t>CREATE INDEX ON LIVE (DELIVERY_DATE);</t>
-  </si>
-  <si>
     <t>ADDRESS</t>
   </si>
   <si>
@@ -377,6 +297,84 @@
   </si>
   <si>
     <t>PRIMARY KEY (ADDRESS)</t>
+  </si>
+  <si>
+    <t>NEXT_SLOT</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (ID)</t>
+  </si>
+  <si>
+    <t>identifier of content: 0-current due slot that SMSC process now, 1-last assigned messageId</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>DUE_SLOT</t>
+  </si>
+  <si>
+    <t>This table contains system general values</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY ("TARGET_ID")</t>
+  </si>
+  <si>
+    <t>This table contains a list for due_slot values of for targetId for storing data for this day.</t>
+  </si>
+  <si>
+    <t>New coming messages will be added into this due_slot if it is not yet already processed.</t>
+  </si>
+  <si>
+    <t>If due_slot is already processed or is absent a new due_slot will be assigned</t>
+  </si>
+  <si>
+    <t>due_slot for which this messages will be loaded for delivering</t>
+  </si>
+  <si>
+    <t>0-idle state, 1-delivering is in progress, 2-delivering is finished (by success or failure)</t>
+  </si>
+  <si>
+    <t>SMSC_UUID</t>
+  </si>
+  <si>
+    <t>Id of SMSC session (from start to stop), we need this to know which session has launched the delivery of a message</t>
+  </si>
+  <si>
+    <t>This field is not used now because this demands extra database access.</t>
+  </si>
+  <si>
+    <t>unique message ID assigned by SMSC</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (("DUE_SLOT"), "TARGET_ID", "ID")</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (("ADDR_DST_DIGITS"), ID);</t>
+  </si>
+  <si>
+    <t>record identifier</t>
+  </si>
+  <si>
+    <t>Here messages that are scheduled for delivering are stored</t>
+  </si>
+  <si>
+    <t>After delivering messages are not deleted</t>
+  </si>
+  <si>
+    <t>This is some sort of archive where sent or delivery failured messages are stored</t>
+  </si>
+  <si>
+    <t>due_slot for which this messages was loaded for delivering</t>
+  </si>
+  <si>
+    <t>do not used in this table</t>
+  </si>
+  <si>
+    <t>duration after which new deliver attempt will be done (in sec) - value before the last delivering attempt</t>
+  </si>
+  <si>
+    <t>ErrorCode value will be put here for last attempt (0==delivered, !=0 – ErrorCode of the last attempt)</t>
   </si>
 </sst>
 </file>
@@ -858,10 +856,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="87.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:IV65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -889,229 +1039,133 @@
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3"/>
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3"/>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3"/>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="3"/>
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A34"/>
+      <selection activeCell="A16" sqref="A1:IV65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -1134,12 +1188,14 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="11" t="s">
@@ -1154,303 +1210,456 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>34</v>
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>35</v>
+      <c r="A14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" t="s">
-        <v>57</v>
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>75</v>
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>77</v>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="11" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="11" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="11" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+      <c r="B39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="B40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="B42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1463,12 +1672,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -1478,7 +1687,7 @@
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1489,438 +1698,473 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="11" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="B9" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="11" t="s">
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="B12" s="11" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="11" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="11" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" t="s">
-        <v>57</v>
+      <c r="A21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>67</v>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="11" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="11" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="11" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="11" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="11" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="11" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>100</v>
+        <v>56</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="11" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="11" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>108</v>
-      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="A40" s="11" t="s">
         <v>84</v>
       </c>
+      <c r="B40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>109</v>
+      <c r="A42" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>111</v>
+      <c r="A43" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1939,13 +2183,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -1966,29 +2208,29 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>